<commit_message>
Added sample files and fixed bug where it was uploading nulls
</commit_message>
<xml_diff>
--- a/testxl.xlsx
+++ b/testxl.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicholas\Documents\work\Architects\timelogs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicholas\Documents\timelog-bot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7969236F-09C5-4E7C-B42A-04E0F41170B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6F44CF0-773A-460A-935D-7F8DA5BE0DB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11385" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="735" yWindow="735" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="day1" sheetId="7" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="25">
   <si>
     <t>Ticket</t>
   </si>
@@ -85,37 +85,7 @@
     <t>ARC-1</t>
   </si>
   <si>
-    <t>Prepped for standup and standup</t>
-  </si>
-  <si>
-    <t>Training</t>
-  </si>
-  <si>
-    <t>Watched videos re: processes</t>
-  </si>
-  <si>
-    <t>Met with Valentine to go over basic ticket and app stuff. Got the app running and db fixed</t>
-  </si>
-  <si>
-    <t>Reviewed app flow and project divisions/processes with Brandon</t>
-  </si>
-  <si>
     <t>ORIG-675</t>
-  </si>
-  <si>
-    <t>Good a good test flow going. Worked on gettign the styles to go through. Read up on sass media queries and learned about RAPID's web architecture</t>
-  </si>
-  <si>
-    <t>Figured out how to get the scss architecture going and got the icons to hide in mobile</t>
-  </si>
-  <si>
-    <t>Prep for standup and standup</t>
-  </si>
-  <si>
-    <t>Reorganized things and got all but the font size and miscellaneous loan similarities in</t>
-  </si>
-  <si>
-    <t>Got the font and select options to look right.  Only thing left should be the undeclared changes</t>
   </si>
   <si>
     <t>Made more components</t>
@@ -143,24 +113,6 @@
   </si>
   <si>
     <t>PR changes and setting up linter</t>
-  </si>
-  <si>
-    <t>Backmerged, linted, fixed vsc settings. Verified with Bharat, and merged in branch</t>
-  </si>
-  <si>
-    <t>Looked into mobile datepicker components and experimented with style changes</t>
-  </si>
-  <si>
-    <t>Updated everything via styles and tested</t>
-  </si>
-  <si>
-    <t>Grooming meeting</t>
-  </si>
-  <si>
-    <t>Deployed to QA, verified on mobile device and sent it to Bharat for approval. Coordinated on next priority</t>
-  </si>
-  <si>
-    <t>Reviewed changes with Bharat and made pr.  Made a couple changes after speaking with him.  Deployed it to QA1 for testing</t>
   </si>
 </sst>
 </file>
@@ -623,7 +575,7 @@
   <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -664,143 +616,84 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="1">
-        <v>0.39583333333333331</v>
-      </c>
-      <c r="C2" s="1">
-        <v>0.41666666666666669</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>15</v>
-      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
       <c r="E2" s="1">
         <f t="shared" ref="E2:E23" si="0">C2-B2</f>
-        <v>2.083333333333337E-2</v>
+        <v>0</v>
       </c>
       <c r="F2" s="1">
         <f>IF(ISBLANK(C2), 0, SUM($E$2:E2))</f>
-        <v>2.083333333333337E-2</v>
+        <v>0</v>
       </c>
       <c r="H2" s="1">
         <f>SUM(E2:E32)</f>
-        <v>0.3229166666666668</v>
+        <v>0</v>
       </c>
       <c r="I2" s="3">
         <f>SUM('day1'!H2,'day2'!H2,'day3'!H2,'day4'!H2,'day5'!H2)</f>
-        <v>1.3645833333333335</v>
+        <v>0.40625</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="1">
-        <v>0.41666666666666669</v>
-      </c>
-      <c r="C3" s="1">
-        <v>0.45833333333333331</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>17</v>
-      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
       <c r="E3" s="1">
         <f t="shared" si="0"/>
-        <v>4.166666666666663E-2</v>
+        <v>0</v>
       </c>
       <c r="F3" s="1">
         <f>IF(ISBLANK(C3), 0, SUM($E$2:E3))</f>
-        <v>6.25E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="1">
-        <v>0.45833333333333331</v>
-      </c>
-      <c r="C4" s="1">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>18</v>
-      </c>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
       <c r="E4" s="1">
         <f t="shared" si="0"/>
-        <v>8.3333333333333315E-2</v>
+        <v>0</v>
       </c>
       <c r="F4" s="1">
         <f>IF(ISBLANK(C4), 0, SUM($E$2:E4))</f>
-        <v>0.14583333333333331</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="1">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="C5" s="1">
-        <v>0.58333333333333337</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>19</v>
-      </c>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
       <c r="E5" s="1">
         <f t="shared" si="0"/>
-        <v>4.1666666666666741E-2</v>
+        <v>0</v>
       </c>
       <c r="F5" s="1">
         <f>IF(ISBLANK(C5), 0, SUM($E$2:E5))</f>
-        <v>0.18750000000000006</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="1">
-        <v>0.69791666666666663</v>
-      </c>
-      <c r="C6" s="1">
-        <v>0.79166666666666663</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>21</v>
-      </c>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
       <c r="E6" s="1">
         <f t="shared" si="0"/>
-        <v>9.375E-2</v>
+        <v>0</v>
       </c>
       <c r="F6" s="1">
         <f>IF(ISBLANK(C6), 0, SUM($E$2:E6))</f>
-        <v>0.28125000000000006</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="1">
-        <v>0.82291666666666663</v>
-      </c>
-      <c r="C7" s="1">
-        <v>0.86458333333333337</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>22</v>
-      </c>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
       <c r="E7" s="1">
         <f t="shared" si="0"/>
-        <v>4.1666666666666741E-2</v>
+        <v>0</v>
       </c>
       <c r="F7" s="1">
         <f>IF(ISBLANK(C7), 0, SUM($E$2:E7))</f>
-        <v>0.3229166666666668</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -1059,7 +952,7 @@
   <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1100,77 +993,49 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="1">
-        <v>0.39583333333333331</v>
-      </c>
-      <c r="C2" s="1">
-        <v>0.41666666666666669</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>23</v>
-      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
       <c r="E2" s="1">
         <f>C2-B2</f>
-        <v>2.083333333333337E-2</v>
+        <v>0</v>
       </c>
       <c r="F2" s="1">
         <f>IF(ISBLANK(C2), 0, SUM($E$2:E2))</f>
-        <v>2.083333333333337E-2</v>
+        <v>0</v>
       </c>
       <c r="H2" s="1">
         <f>SUM(E2:E32)</f>
-        <v>0.33333333333333348</v>
+        <v>0</v>
       </c>
       <c r="I2" s="3">
         <f>SUM('day1'!H2,'day2'!H2,'day3'!H2,'day4'!H2,'day5'!H2)</f>
-        <v>1.3645833333333335</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" s="1">
-        <v>0.4375</v>
-      </c>
-      <c r="C3" s="1">
-        <v>0.64583333333333337</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>24</v>
-      </c>
+        <v>0.40625</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="5"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
       <c r="E3" s="1">
         <f>C3-B3</f>
-        <v>0.20833333333333337</v>
+        <v>0</v>
       </c>
       <c r="F3" s="1">
         <f>IF(ISBLANK(C3), 0, SUM($E$2:E3))</f>
-        <v>0.22916666666666674</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" s="1">
-        <v>0.85416666666666663</v>
-      </c>
-      <c r="C4" s="1">
-        <v>0.95833333333333337</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>25</v>
-      </c>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
       <c r="E4" s="1">
         <f t="shared" ref="E4:E22" si="0">C4-B4</f>
-        <v>0.10416666666666674</v>
+        <v>0</v>
       </c>
       <c r="F4" s="1">
         <f>IF(ISBLANK(C4), 0, SUM($E$2:E4))</f>
-        <v>0.33333333333333348</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -1465,8 +1330,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1518,10 +1383,10 @@
         <v>6.25E-2</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="E2" s="1">
-        <f>C2-B2</f>
+        <f t="shared" ref="E2:E26" si="0">C2-B2</f>
         <v>2.0833333333333336E-2</v>
       </c>
       <c r="F2" s="1">
@@ -1534,7 +1399,7 @@
       </c>
       <c r="I2" s="3">
         <f>SUM('day1'!H2,'day2'!H2,'day3'!H2,'day4'!H2,'day5'!H2)</f>
-        <v>1.3645833333333335</v>
+        <v>0.40625</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -1551,7 +1416,7 @@
         <v>13</v>
       </c>
       <c r="E3" s="1">
-        <f>C3-B3</f>
+        <f t="shared" si="0"/>
         <v>1.0416666666666685E-2</v>
       </c>
       <c r="F3" s="1">
@@ -1570,10 +1435,10 @@
         <v>0.54166666666666663</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="E4" s="1">
-        <f>C4-B4</f>
+        <f t="shared" si="0"/>
         <v>0.12499999999999994</v>
       </c>
       <c r="F4" s="1">
@@ -1583,7 +1448,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B5" s="1">
         <v>0.55208333333333337</v>
@@ -1592,10 +1457,10 @@
         <v>0.59375</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="E5" s="1">
-        <f>C5-B5</f>
+        <f t="shared" si="0"/>
         <v>4.166666666666663E-2</v>
       </c>
       <c r="F5" s="1">
@@ -1614,10 +1479,10 @@
         <v>0.64583333333333337</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="E6" s="1">
-        <f>C6-B6</f>
+        <f t="shared" si="0"/>
         <v>5.208333333333337E-2</v>
       </c>
       <c r="F6" s="1">
@@ -1627,7 +1492,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B7" s="1">
         <v>0.64583333333333337</v>
@@ -1636,10 +1501,10 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="E7" s="1">
-        <f>C7-B7</f>
+        <f t="shared" si="0"/>
         <v>6.25E-2</v>
       </c>
       <c r="F7" s="1">
@@ -1649,7 +1514,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B8" s="1">
         <v>0.83333333333333337</v>
@@ -1658,10 +1523,10 @@
         <v>0.84375</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="E8" s="1">
-        <f>C8-B8</f>
+        <f t="shared" si="0"/>
         <v>1.041666666666663E-2</v>
       </c>
       <c r="F8" s="1">
@@ -1673,7 +1538,7 @@
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="E9" s="1">
-        <f>C9-B9</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F9" s="1">
@@ -1685,7 +1550,7 @@
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="E10" s="1">
-        <f>C10-B10</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F10" s="1">
@@ -1697,7 +1562,7 @@
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="E11" s="1">
-        <f>C11-B11</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F11" s="1">
@@ -1709,7 +1574,7 @@
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="E12" s="1">
-        <f>C12-B12</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F12" s="1">
@@ -1722,7 +1587,7 @@
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="E13" s="1">
-        <f>C13-B13</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F13" s="1">
@@ -1734,7 +1599,7 @@
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="E14" s="1">
-        <f>C14-B14</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F14" s="1">
@@ -1746,7 +1611,7 @@
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="E15" s="1">
-        <f>C15-B15</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F15" s="1">
@@ -1758,7 +1623,7 @@
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="E16" s="1">
-        <f>C16-B16</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F16" s="1">
@@ -1770,7 +1635,7 @@
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="E17" s="1">
-        <f>C17-B17</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F17" s="1">
@@ -1782,7 +1647,7 @@
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="E18" s="1">
-        <f>C18-B18</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F18" s="1">
@@ -1794,7 +1659,7 @@
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="E19" s="1">
-        <f>C19-B19</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F19" s="1">
@@ -1806,7 +1671,7 @@
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="E20" s="1">
-        <f>C20-B20</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F20" s="1">
@@ -1818,7 +1683,7 @@
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="E21" s="1">
-        <f>C21-B21</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F21" s="1">
@@ -1828,7 +1693,7 @@
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E22" s="1">
-        <f>C22-B22</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F22" s="1">
@@ -1838,7 +1703,7 @@
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E23" s="1">
-        <f>C23-B23</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F23" s="1">
@@ -1848,7 +1713,7 @@
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E24" s="1">
-        <f>C24-B24</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F24" s="1">
@@ -1858,7 +1723,7 @@
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E25" s="1">
-        <f>C25-B25</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F25" s="1">
@@ -1868,7 +1733,7 @@
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E26" s="1">
-        <f>C26-B26</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F26" s="1">
@@ -1899,8 +1764,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1943,7 +1808,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="B2" s="1">
         <v>0.33333333333333331</v>
@@ -1952,7 +1817,7 @@
         <v>0.375</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="E2" s="1">
         <f>C2-B2</f>
@@ -1964,16 +1829,16 @@
       </c>
       <c r="H2" s="1">
         <f>SUM(E2:E32)</f>
-        <v>0.38541666666666663</v>
+        <v>8.333333333333337E-2</v>
       </c>
       <c r="I2" s="3">
         <f>SUM('day1'!H2,'day2'!H2,'day3'!H2,'day4'!H2,'day5'!H2)</f>
-        <v>1.3645833333333335</v>
+        <v>0.40625</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B3" s="1">
         <v>0.375</v>
@@ -1982,7 +1847,7 @@
         <v>0.40625</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="E3" s="1">
         <f>C3-B3</f>
@@ -2015,136 +1880,82 @@
         <v>8.333333333333337E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" s="1">
-        <v>0.41666666666666669</v>
-      </c>
-      <c r="C5" s="1">
-        <v>0.45833333333333331</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>35</v>
-      </c>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
       <c r="E5" s="1">
         <f>C5-B5</f>
-        <v>4.166666666666663E-2</v>
+        <v>0</v>
       </c>
       <c r="F5" s="1">
         <f>IF(ISBLANK(C5), 0, SUM($E$2:E5))</f>
-        <v>0.125</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B6" s="1">
-        <v>0.46875</v>
-      </c>
-      <c r="C6" s="1">
-        <v>0.51041666666666663</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>36</v>
-      </c>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
       <c r="E6" s="1">
         <f t="shared" ref="E6:E28" si="0">C6-B6</f>
-        <v>4.166666666666663E-2</v>
+        <v>0</v>
       </c>
       <c r="F6" s="1">
         <f>IF(ISBLANK(C6), 0, SUM($E$2:E6))</f>
-        <v>0.16666666666666663</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B7" s="1">
-        <v>0.53125</v>
-      </c>
-      <c r="C7" s="1">
-        <v>0.625</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>37</v>
-      </c>
+      <c r="A7" s="2"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
       <c r="E7" s="1">
         <f t="shared" si="0"/>
-        <v>9.375E-2</v>
+        <v>0</v>
       </c>
       <c r="F7" s="1">
         <f>IF(ISBLANK(C7), 0, SUM($E$2:E7))</f>
-        <v>0.26041666666666663</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="1">
-        <v>0.625</v>
-      </c>
-      <c r="C8" s="1">
-        <v>0.65625</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>38</v>
-      </c>
+      <c r="A8" s="2"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
       <c r="E8" s="1">
         <f t="shared" si="0"/>
-        <v>3.125E-2</v>
+        <v>0</v>
       </c>
       <c r="F8" s="1">
         <f>IF(ISBLANK(C8), 0, SUM($E$2:E8))</f>
-        <v>0.29166666666666663</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B9" s="1">
-        <v>0.65625</v>
-      </c>
-      <c r="C9" s="1">
-        <v>0.6875</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>39</v>
-      </c>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
       <c r="E9" s="1">
         <f t="shared" si="0"/>
-        <v>3.125E-2</v>
+        <v>0</v>
       </c>
       <c r="F9" s="1">
         <f>IF(ISBLANK(C9), 0, SUM($E$2:E9))</f>
-        <v>0.32291666666666663</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10" s="1">
-        <v>0.69791666666666663</v>
-      </c>
-      <c r="C10" s="1">
-        <v>0.76041666666666663</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>40</v>
-      </c>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
       <c r="E10" s="1">
         <f t="shared" si="0"/>
-        <v>6.25E-2</v>
+        <v>0</v>
       </c>
       <c r="F10" s="1">
         <f>IF(ISBLANK(C10), 0, SUM($E$2:E10))</f>
-        <v>0.38541666666666663</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -2387,7 +2198,7 @@
   <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D5"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2444,7 +2255,7 @@
       </c>
       <c r="I2" s="3">
         <f>SUM('day1'!H2,'day2'!H2,'day3'!H2,'day4'!H2,'day5'!H2)</f>
-        <v>1.3645833333333335</v>
+        <v>0.40625</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>